<commit_message>
Replace day-12.xlsx with updated version
</commit_message>
<xml_diff>
--- a/Data-Analytics-Excel Files/day-12.xlsx
+++ b/Data-Analytics-Excel Files/day-12.xlsx
@@ -5,17 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sonal Kshirsagar\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sonal Kshirsagar\Desktop\Data Analytics\ARC Technology\Excel\Data-Analytics-Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D6BF05-6132-4532-AE6B-22200EF64716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900965CB-F31E-40D5-9407-25255CF291A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="basic" sheetId="2" r:id="rId1"/>
     <sheet name="VLOOKUP" sheetId="14" r:id="rId2"/>
     <sheet name="HLOOKUP" sheetId="15" r:id="rId3"/>
+    <sheet name="Index" sheetId="16" r:id="rId4"/>
+    <sheet name="Match" sheetId="17" r:id="rId5"/>
+    <sheet name="index match" sheetId="18" r:id="rId6"/>
+    <sheet name="Xlookup" sheetId="19" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="58">
   <si>
     <t>ARC</t>
   </si>
@@ -180,6 +184,27 @@
   </si>
   <si>
     <t>Formula</t>
+  </si>
+  <si>
+    <t>row_num</t>
+  </si>
+  <si>
+    <t>col_num</t>
+  </si>
+  <si>
+    <t>index_num</t>
+  </si>
+  <si>
+    <t>index_row</t>
+  </si>
+  <si>
+    <t>index_col</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>automotive sq</t>
   </si>
 </sst>
 </file>
@@ -375,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -385,13 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -400,44 +419,28 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -611,25 +614,51 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -646,16 +675,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9653A1E6-ADD4-45FE-9334-E921D27B7879}" name="Table1" displayName="Table1" ref="C6:I12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9653A1E6-ADD4-45FE-9334-E921D27B7879}" name="Table1" displayName="Table1" ref="C6:I12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="C6:I12" xr:uid="{9653A1E6-ADD4-45FE-9334-E921D27B7879}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4A071E0F-BD66-427B-9C83-D61260E5A25D}" name="shop_name" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{3CF1E6B7-AC9C-4764-9374-EC37460B792F}" name="address" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{CD0AA6F9-CE1F-4DAD-AEC1-63A82B2AAECE}" name="mode" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{ACD6A26B-05C8-4447-A8FF-8D6673376D50}" name="Outlet" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{1B110E94-1D3A-4806-9B7A-75E521E5FC33}" name="customer_count" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{66A6CA15-9274-477D-A0F5-14AE617DF0A7}" name="sales" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{D75C365A-C3A8-4411-A381-53282AFD39FA}" name="employee" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{4A071E0F-BD66-427B-9C83-D61260E5A25D}" name="shop_name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{3CF1E6B7-AC9C-4764-9374-EC37460B792F}" name="address" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{CD0AA6F9-CE1F-4DAD-AEC1-63A82B2AAECE}" name="mode" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{ACD6A26B-05C8-4447-A8FF-8D6673376D50}" name="Outlet" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1B110E94-1D3A-4806-9B7A-75E521E5FC33}" name="customer_count" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{66A6CA15-9274-477D-A0F5-14AE617DF0A7}" name="sales" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{D75C365A-C3A8-4411-A381-53282AFD39FA}" name="employee" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1049,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A40DD5A-2EA0-453B-B205-8D25B7B6EF10}">
   <dimension ref="C2:Q21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6:Q11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,15 +1096,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
     </row>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O3" t="s">
@@ -1119,7 +1148,7 @@
       <c r="P5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="Q5" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1134,7 +1163,7 @@
         <v>39</v>
       </c>
       <c r="G6" s="1">
-        <f>VLOOKUP($D6,$L$5:$M$11,2,FALSE)</f>
+        <f t="shared" ref="G6:G11" si="0">VLOOKUP($D6,$L$5:$M$11,2,FALSE)</f>
         <v>5</v>
       </c>
       <c r="H6" s="5">
@@ -1164,7 +1193,7 @@
         <v>1000</v>
       </c>
       <c r="Q6" s="1">
-        <f t="shared" ref="Q6:Q10" si="0">VLOOKUP(L6,$D$5:$J$11,7,FALSE)</f>
+        <f t="shared" ref="Q6:Q10" si="1">VLOOKUP(L6,$D$5:$J$11,7,FALSE)</f>
         <v>700</v>
       </c>
     </row>
@@ -1179,7 +1208,7 @@
         <v>39</v>
       </c>
       <c r="G7" s="1">
-        <f>VLOOKUP($D7,$L$5:$M$11,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H7" s="5">
@@ -1189,7 +1218,7 @@
         <v>10000</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" ref="J7:J11" si="1">VLOOKUP(D7,$L$5:$O$11,4,FALSE)</f>
+        <f t="shared" ref="J7:J11" si="2">VLOOKUP(D7,$L$5:$O$11,4,FALSE)</f>
         <v>700</v>
       </c>
       <c r="L7" s="5" t="s">
@@ -1205,11 +1234,11 @@
         <v>100</v>
       </c>
       <c r="P7" s="1">
-        <f t="shared" ref="P7:P11" si="2">VLOOKUP(L7,$D$5:$J$11,5,FALSE)</f>
+        <f t="shared" ref="P7:P11" si="3">VLOOKUP(L7,$D$5:$J$11,5,FALSE)</f>
         <v>15000</v>
       </c>
       <c r="Q7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1224,7 +1253,7 @@
         <v>39</v>
       </c>
       <c r="G8" s="1">
-        <f>VLOOKUP($D8,$L$5:$M$11,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H8" s="5">
@@ -1234,7 +1263,7 @@
         <v>200000</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5000</v>
       </c>
       <c r="L8" s="5" t="s">
@@ -1250,7 +1279,7 @@
         <v>1000</v>
       </c>
       <c r="P8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2000</v>
       </c>
       <c r="Q8" s="1">
@@ -1269,7 +1298,7 @@
         <v>40</v>
       </c>
       <c r="G9" s="1">
-        <f>VLOOKUP($D9,$L$5:$M$11,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H9" s="5">
@@ -1279,7 +1308,7 @@
         <v>200000</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="L9" s="5" t="s">
@@ -1295,11 +1324,11 @@
         <v>5000</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7000</v>
       </c>
       <c r="Q9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
     </row>
@@ -1314,7 +1343,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="1">
-        <f>VLOOKUP($D10,$L$5:$M$11,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H10" s="5">
@@ -1324,7 +1353,7 @@
         <v>150000</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="L10" s="5" t="s">
@@ -1340,11 +1369,11 @@
         <v>7000</v>
       </c>
       <c r="P10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
       <c r="Q10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7000</v>
       </c>
     </row>
@@ -1359,7 +1388,7 @@
         <v>39</v>
       </c>
       <c r="G11" s="1">
-        <f>VLOOKUP($D11,$L$5:$M$11,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="H11" s="5">
@@ -1369,7 +1398,7 @@
         <v>50000</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="L11" s="5" t="s">
@@ -1385,7 +1414,7 @@
         <v>20</v>
       </c>
       <c r="P11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12000</v>
       </c>
       <c r="Q11" s="1">
@@ -1415,7 +1444,7 @@
       <c r="K15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="8"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" spans="3:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
@@ -1425,14 +1454,14 @@
         <v>39</v>
       </c>
       <c r="E16" s="1">
-        <f>VLOOKUP($C16,$D$5:$O$11,6,FALSE)</f>
+        <f t="shared" ref="E16:E21" si="4">VLOOKUP($C16,$D$5:$O$11,6,FALSE)</f>
         <v>100000</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>VLOOKUP(G16,$D$5:$O$11,3,FALSE)</f>
+        <f t="shared" ref="H16:H21" si="5">VLOOKUP(G16,$D$5:$O$11,3,FALSE)</f>
         <v>offline</v>
       </c>
       <c r="J16" s="5" t="s">
@@ -1450,14 +1479,14 @@
         <v>40</v>
       </c>
       <c r="E17" s="1">
-        <f>VLOOKUP($C17,$D$5:$O$11,6,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>150000</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>29</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>VLOOKUP(G17,$D$5:$O$11,3,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>online</v>
       </c>
       <c r="J17" s="5" t="s">
@@ -1475,14 +1504,14 @@
         <v>39</v>
       </c>
       <c r="E18" s="1">
-        <f>VLOOKUP($C18,$D$5:$O$11,6,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>50000</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>VLOOKUP(G18,$D$5:$O$11,3,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>offline</v>
       </c>
       <c r="J18" s="5" t="s">
@@ -1500,17 +1529,17 @@
         <v>39</v>
       </c>
       <c r="E19" s="1">
-        <f>VLOOKUP($C19,$D$5:$O$11,6,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>200000</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>VLOOKUP(G19,$D$5:$O$11,3,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>offline</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="6" t="s">
         <v>45</v>
       </c>
       <c r="K19" s="5" t="s">
@@ -1525,14 +1554,14 @@
         <v>39</v>
       </c>
       <c r="E20" s="1">
-        <f>VLOOKUP($C20,$D$5:$O$11,6,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>10000</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>VLOOKUP(G20,$D$5:$O$11,3,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>offline</v>
       </c>
       <c r="J20" s="5" t="s">
@@ -1550,14 +1579,14 @@
         <v>40</v>
       </c>
       <c r="E21" s="1">
-        <f>VLOOKUP($C21,$D$5:$O$11,6,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>200000</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>28</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>VLOOKUP(G21,$D$5:$O$11,3,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>online</v>
       </c>
       <c r="J21" s="5" t="s">
@@ -1579,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBC2DCD-5418-4655-A853-06C1D80E8282}">
   <dimension ref="A3:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,52 +1626,52 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1660,12 +1689,12 @@
       <c r="H7" s="5">
         <v>100000</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="9">
         <v>700</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -1683,12 +1712,12 @@
       <c r="H8" s="5">
         <v>10000</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="9">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1706,12 +1735,12 @@
       <c r="H9" s="5">
         <v>200000</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="9">
         <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1729,7 +1758,7 @@
       <c r="H10" s="5">
         <v>200000</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="9">
         <v>5000</v>
       </c>
       <c r="K10" s="4" t="s">
@@ -1752,7 +1781,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="75" x14ac:dyDescent="0.25">
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1770,7 +1799,7 @@
       <c r="H11" s="5">
         <v>150000</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="9">
         <v>7000</v>
       </c>
       <c r="K11" s="6" t="s">
@@ -1793,25 +1822,25 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="16">
+      <c r="E12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="14">
         <v>10</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="14">
         <v>2000</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="14">
         <v>50000</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="15">
         <v>20</v>
       </c>
       <c r="K12" s="5" t="s">
@@ -1944,7 +1973,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" ref="E17:H17" si="0">HLOOKUP(F16,$C$6:$I$12,2,FALSE)</f>
+        <f t="shared" ref="F17:H17" si="0">HLOOKUP(F16,$C$6:$I$12,2,FALSE)</f>
         <v>5000</v>
       </c>
       <c r="G17" s="1">
@@ -1997,7 +2026,7 @@
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="1" t="str">
@@ -2030,4 +2059,856 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8CDD51-D305-4150-9E60-205ADB4FFDE8}">
+  <dimension ref="B4:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="H6" s="5">
+        <v>100000</v>
+      </c>
+      <c r="I6" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H7" s="5">
+        <v>10000</v>
+      </c>
+      <c r="I7" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5">
+        <v>7000</v>
+      </c>
+      <c r="H8" s="5">
+        <v>200000</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>15000</v>
+      </c>
+      <c r="H9" s="5">
+        <v>200000</v>
+      </c>
+      <c r="I9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="5">
+        <v>12000</v>
+      </c>
+      <c r="H10" s="5">
+        <v>150000</v>
+      </c>
+      <c r="I10" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2000</v>
+      </c>
+      <c r="H11" s="5">
+        <v>50000</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C13" t="e">
+        <f>INDEX(C5:I11,C8,F5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F14" s="19">
+        <v>5</v>
+      </c>
+      <c r="G14" s="20">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <f>INDEX(C5:I11,F14,G14)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E59047-69F5-4A74-B268-41B8040A3AE7}">
+  <dimension ref="A4:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="22">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5000</v>
+      </c>
+      <c r="G5" s="5">
+        <v>100000</v>
+      </c>
+      <c r="H5" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="22">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1000</v>
+      </c>
+      <c r="G6" s="5">
+        <v>10000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="22">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5">
+        <v>7000</v>
+      </c>
+      <c r="G7" s="5">
+        <v>200000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="22">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>15000</v>
+      </c>
+      <c r="G8" s="5">
+        <v>200000</v>
+      </c>
+      <c r="H8" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="22">
+        <v>3</v>
+      </c>
+      <c r="F9" s="5">
+        <v>12000</v>
+      </c>
+      <c r="G9" s="5">
+        <v>150000</v>
+      </c>
+      <c r="H9" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="22">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5">
+        <v>2000</v>
+      </c>
+      <c r="G10" s="5">
+        <v>50000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <f>MATCH(A13,B4:B10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13">
+        <f>MATCH(F13,D4:D10,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="23">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <f>MATCH(F14,E4:E10,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962BCA45-CFEC-4FAD-8D85-7DA327E1E780}">
+  <dimension ref="C5:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="22">
+        <v>5</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="H6" s="5">
+        <v>100000</v>
+      </c>
+      <c r="I6" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="22">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H7" s="5">
+        <v>10000</v>
+      </c>
+      <c r="I7" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="22">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5">
+        <v>7000</v>
+      </c>
+      <c r="H8" s="5">
+        <v>200000</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="22">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>15000</v>
+      </c>
+      <c r="H9" s="5">
+        <v>200000</v>
+      </c>
+      <c r="I9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="22">
+        <v>3</v>
+      </c>
+      <c r="G10" s="5">
+        <v>12000</v>
+      </c>
+      <c r="H10" s="5">
+        <v>150000</v>
+      </c>
+      <c r="I10" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="22">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2000</v>
+      </c>
+      <c r="H11" s="5">
+        <v>50000</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <f>INDEX(C5:I11,E14,E15)</f>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15">
+        <f>MATCH(D15,C5:I5,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFDC74A8-5230-496A-92D0-3B93596461BA}">
+  <dimension ref="D5:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="22">
+        <v>5</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="I6" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J6" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="22">
+        <v>2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1000</v>
+      </c>
+      <c r="I7" s="5">
+        <v>10000</v>
+      </c>
+      <c r="J7" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="22">
+        <v>6</v>
+      </c>
+      <c r="H8" s="5">
+        <v>7000</v>
+      </c>
+      <c r="I8" s="5">
+        <v>200000</v>
+      </c>
+      <c r="J8" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="22">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>15000</v>
+      </c>
+      <c r="I9" s="5">
+        <v>200000</v>
+      </c>
+      <c r="J9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="22">
+        <v>3</v>
+      </c>
+      <c r="H10" s="5">
+        <v>12000</v>
+      </c>
+      <c r="I10" s="5">
+        <v>150000</v>
+      </c>
+      <c r="J10" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="22">
+        <v>10</v>
+      </c>
+      <c r="H11" s="5">
+        <v>2000</v>
+      </c>
+      <c r="I11" s="5">
+        <v>50000</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E15" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>